<commit_message>
Pre data generation. Still not yet geenrated. Setting up parameters for data generation
</commit_message>
<xml_diff>
--- a/data/home.xlsx
+++ b/data/home.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EDDA0591-BDA8-44BE-893B-994BF5D2AE75}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3B61BDDF-0993-48B4-9036-23E4AD6B184D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -412,7 +412,7 @@
   <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N5" sqref="K5:N13"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Created home database of priorities
</commit_message>
<xml_diff>
--- a/data/home.xlsx
+++ b/data/home.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EE596EA6-085A-4B05-A516-21097C81F440}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{75F2E4A7-5606-4CAF-A96F-CC52082BE94B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="47">
   <si>
     <t>device</t>
   </si>
@@ -160,9 +160,6 @@
   </si>
   <si>
     <t>midnight</t>
-  </si>
-  <si>
-    <t>priotiy</t>
   </si>
   <si>
     <t>order</t>
@@ -1529,10 +1526,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A55FD11-B1DA-4CBF-9482-8027348840F6}">
-  <dimension ref="A1:Q37"/>
+  <dimension ref="A1:E109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="66" workbookViewId="0">
-      <selection activeCell="T18" sqref="T18"/>
+    <sheetView tabSelected="1" zoomScale="62" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1547,7 +1544,7 @@
     <col min="15" max="15" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1561,40 +1558,10 @@
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="P1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1610,38 +1577,8 @@
       <c r="E2">
         <v>52</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J2">
-        <v>7</v>
-      </c>
-      <c r="K2">
-        <v>42</v>
-      </c>
-      <c r="M2" t="s">
-        <v>21</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="O2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P2">
-        <v>10</v>
-      </c>
-      <c r="Q2">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1657,38 +1594,8 @@
       <c r="E3">
         <v>49</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3">
-        <v>7</v>
-      </c>
-      <c r="K3">
-        <v>43</v>
-      </c>
-      <c r="M3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="O3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P3">
-        <v>13</v>
-      </c>
-      <c r="Q3">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1704,38 +1611,8 @@
       <c r="E4">
         <v>48</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4">
-        <v>7</v>
-      </c>
-      <c r="K4">
-        <v>44</v>
-      </c>
-      <c r="M4" t="s">
-        <v>21</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="O4" t="s">
-        <v>23</v>
-      </c>
-      <c r="P4">
-        <v>17</v>
-      </c>
-      <c r="Q4">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1751,38 +1628,8 @@
       <c r="E5">
         <v>50</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5">
-        <v>7</v>
-      </c>
-      <c r="K5">
-        <v>45</v>
-      </c>
-      <c r="M5" t="s">
-        <v>21</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="O5" t="s">
-        <v>22</v>
-      </c>
-      <c r="P5">
-        <v>14</v>
-      </c>
-      <c r="Q5">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1798,38 +1645,8 @@
       <c r="E6">
         <v>51</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6">
-        <v>7</v>
-      </c>
-      <c r="K6">
-        <v>46</v>
-      </c>
-      <c r="M6" t="s">
-        <v>21</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="O6" t="s">
-        <v>24</v>
-      </c>
-      <c r="P6">
-        <v>1</v>
-      </c>
-      <c r="Q6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1845,38 +1662,8 @@
       <c r="E7">
         <v>53</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" t="s">
-        <v>45</v>
-      </c>
-      <c r="J7">
-        <v>7</v>
-      </c>
-      <c r="K7">
-        <v>47</v>
-      </c>
-      <c r="M7" t="s">
-        <v>21</v>
-      </c>
-      <c r="N7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="O7" t="s">
-        <v>45</v>
-      </c>
-      <c r="P7">
-        <v>1</v>
-      </c>
-      <c r="Q7">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -1892,38 +1679,8 @@
       <c r="E8">
         <v>70</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" t="s">
-        <v>44</v>
-      </c>
-      <c r="J8">
-        <v>5</v>
-      </c>
-      <c r="K8">
-        <v>31</v>
-      </c>
-      <c r="M8" t="s">
-        <v>21</v>
-      </c>
-      <c r="N8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="O8" t="s">
-        <v>44</v>
-      </c>
-      <c r="P8">
-        <v>10</v>
-      </c>
-      <c r="Q8">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1939,38 +1696,8 @@
       <c r="E9">
         <v>67</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" t="s">
-        <v>25</v>
-      </c>
-      <c r="J9">
-        <v>5</v>
-      </c>
-      <c r="K9">
-        <v>32</v>
-      </c>
-      <c r="M9" t="s">
-        <v>21</v>
-      </c>
-      <c r="N9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="O9" t="s">
-        <v>25</v>
-      </c>
-      <c r="P9">
-        <v>13</v>
-      </c>
-      <c r="Q9">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -1986,38 +1713,8 @@
       <c r="E10">
         <v>66</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J10">
-        <v>5</v>
-      </c>
-      <c r="K10">
-        <v>33</v>
-      </c>
-      <c r="M10" t="s">
-        <v>21</v>
-      </c>
-      <c r="N10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="O10" t="s">
-        <v>23</v>
-      </c>
-      <c r="P10">
-        <v>17</v>
-      </c>
-      <c r="Q10">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -2033,38 +1730,8 @@
       <c r="E11">
         <v>68</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I11" t="s">
-        <v>22</v>
-      </c>
-      <c r="J11">
-        <v>5</v>
-      </c>
-      <c r="K11">
-        <v>34</v>
-      </c>
-      <c r="M11" t="s">
-        <v>21</v>
-      </c>
-      <c r="N11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="O11" t="s">
-        <v>22</v>
-      </c>
-      <c r="P11">
-        <v>14</v>
-      </c>
-      <c r="Q11">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -2080,38 +1747,8 @@
       <c r="E12">
         <v>69</v>
       </c>
-      <c r="G12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I12" t="s">
-        <v>24</v>
-      </c>
-      <c r="J12">
-        <v>5</v>
-      </c>
-      <c r="K12">
-        <v>35</v>
-      </c>
-      <c r="M12" t="s">
-        <v>21</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="O12" t="s">
-        <v>24</v>
-      </c>
-      <c r="P12">
-        <v>1</v>
-      </c>
-      <c r="Q12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -2127,38 +1764,8 @@
       <c r="E13">
         <v>71</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I13" t="s">
-        <v>45</v>
-      </c>
-      <c r="J13">
-        <v>5</v>
-      </c>
-      <c r="K13">
-        <v>36</v>
-      </c>
-      <c r="M13" t="s">
-        <v>21</v>
-      </c>
-      <c r="N13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="O13" t="s">
-        <v>45</v>
-      </c>
-      <c r="P13">
-        <v>1</v>
-      </c>
-      <c r="Q13">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -2174,38 +1781,8 @@
       <c r="E14">
         <v>100</v>
       </c>
-      <c r="G14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I14" t="s">
-        <v>44</v>
-      </c>
-      <c r="J14">
-        <v>3</v>
-      </c>
-      <c r="K14">
-        <v>19</v>
-      </c>
-      <c r="M14" t="s">
-        <v>21</v>
-      </c>
-      <c r="N14" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="O14" t="s">
-        <v>44</v>
-      </c>
-      <c r="P14">
-        <v>10</v>
-      </c>
-      <c r="Q14">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -2221,38 +1798,8 @@
       <c r="E15">
         <v>97</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I15" t="s">
-        <v>25</v>
-      </c>
-      <c r="J15">
-        <v>3</v>
-      </c>
-      <c r="K15">
-        <v>20</v>
-      </c>
-      <c r="M15" t="s">
-        <v>21</v>
-      </c>
-      <c r="N15" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="O15" t="s">
-        <v>25</v>
-      </c>
-      <c r="P15">
-        <v>13</v>
-      </c>
-      <c r="Q15">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -2268,38 +1815,8 @@
       <c r="E16">
         <v>96</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I16" t="s">
-        <v>23</v>
-      </c>
-      <c r="J16">
-        <v>3</v>
-      </c>
-      <c r="K16">
-        <v>21</v>
-      </c>
-      <c r="M16" t="s">
-        <v>21</v>
-      </c>
-      <c r="N16" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="O16" t="s">
-        <v>23</v>
-      </c>
-      <c r="P16">
-        <v>17</v>
-      </c>
-      <c r="Q16">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -2315,38 +1832,8 @@
       <c r="E17">
         <v>98</v>
       </c>
-      <c r="G17" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I17" t="s">
-        <v>22</v>
-      </c>
-      <c r="J17">
-        <v>3</v>
-      </c>
-      <c r="K17">
-        <v>22</v>
-      </c>
-      <c r="M17" t="s">
-        <v>21</v>
-      </c>
-      <c r="N17" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="O17" t="s">
-        <v>22</v>
-      </c>
-      <c r="P17">
-        <v>14</v>
-      </c>
-      <c r="Q17">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -2362,38 +1849,8 @@
       <c r="E18">
         <v>99</v>
       </c>
-      <c r="G18" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I18" t="s">
-        <v>24</v>
-      </c>
-      <c r="J18">
-        <v>3</v>
-      </c>
-      <c r="K18">
-        <v>23</v>
-      </c>
-      <c r="M18" t="s">
-        <v>21</v>
-      </c>
-      <c r="N18" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="O18" t="s">
-        <v>24</v>
-      </c>
-      <c r="P18">
-        <v>1</v>
-      </c>
-      <c r="Q18">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -2409,38 +1866,8 @@
       <c r="E19">
         <v>101</v>
       </c>
-      <c r="G19" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I19" t="s">
-        <v>45</v>
-      </c>
-      <c r="J19">
-        <v>3</v>
-      </c>
-      <c r="K19">
-        <v>24</v>
-      </c>
-      <c r="M19" t="s">
-        <v>21</v>
-      </c>
-      <c r="N19" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="O19" t="s">
-        <v>45</v>
-      </c>
-      <c r="P19">
-        <v>1</v>
-      </c>
-      <c r="Q19">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -2456,38 +1883,8 @@
       <c r="E20">
         <v>41</v>
       </c>
-      <c r="G20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I20" t="s">
-        <v>44</v>
-      </c>
-      <c r="J20">
-        <v>9</v>
-      </c>
-      <c r="K20">
-        <v>54</v>
-      </c>
-      <c r="M20" t="s">
-        <v>21</v>
-      </c>
-      <c r="N20" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="O20" t="s">
-        <v>44</v>
-      </c>
-      <c r="P20">
-        <v>10</v>
-      </c>
-      <c r="Q20">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -2503,38 +1900,8 @@
       <c r="E21">
         <v>38</v>
       </c>
-      <c r="G21" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I21" t="s">
-        <v>25</v>
-      </c>
-      <c r="J21">
-        <v>9</v>
-      </c>
-      <c r="K21">
-        <v>55</v>
-      </c>
-      <c r="M21" t="s">
-        <v>21</v>
-      </c>
-      <c r="N21" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="O21" t="s">
-        <v>25</v>
-      </c>
-      <c r="P21">
-        <v>13</v>
-      </c>
-      <c r="Q21">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -2550,38 +1917,8 @@
       <c r="E22">
         <v>37</v>
       </c>
-      <c r="G22" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I22" t="s">
-        <v>23</v>
-      </c>
-      <c r="J22">
-        <v>9</v>
-      </c>
-      <c r="K22">
-        <v>56</v>
-      </c>
-      <c r="M22" t="s">
-        <v>21</v>
-      </c>
-      <c r="N22" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="O22" t="s">
-        <v>23</v>
-      </c>
-      <c r="P22">
-        <v>17</v>
-      </c>
-      <c r="Q22">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -2597,38 +1934,8 @@
       <c r="E23">
         <v>39</v>
       </c>
-      <c r="G23" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I23" t="s">
-        <v>22</v>
-      </c>
-      <c r="J23">
-        <v>9</v>
-      </c>
-      <c r="K23">
-        <v>57</v>
-      </c>
-      <c r="M23" t="s">
-        <v>21</v>
-      </c>
-      <c r="N23" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="O23" t="s">
-        <v>22</v>
-      </c>
-      <c r="P23">
-        <v>14</v>
-      </c>
-      <c r="Q23">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -2644,38 +1951,8 @@
       <c r="E24">
         <v>40</v>
       </c>
-      <c r="G24" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I24" t="s">
-        <v>24</v>
-      </c>
-      <c r="J24">
-        <v>9</v>
-      </c>
-      <c r="K24">
-        <v>58</v>
-      </c>
-      <c r="M24" t="s">
-        <v>21</v>
-      </c>
-      <c r="N24" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="O24" t="s">
-        <v>24</v>
-      </c>
-      <c r="P24">
-        <v>1</v>
-      </c>
-      <c r="Q24">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -2691,38 +1968,8 @@
       <c r="E25">
         <v>42</v>
       </c>
-      <c r="G25" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I25" t="s">
-        <v>45</v>
-      </c>
-      <c r="J25">
-        <v>9</v>
-      </c>
-      <c r="K25">
-        <v>59</v>
-      </c>
-      <c r="M25" t="s">
-        <v>21</v>
-      </c>
-      <c r="N25" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="O25" t="s">
-        <v>45</v>
-      </c>
-      <c r="P25">
-        <v>1</v>
-      </c>
-      <c r="Q25">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -2738,38 +1985,8 @@
       <c r="E26">
         <v>29</v>
       </c>
-      <c r="G26" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I26" t="s">
-        <v>44</v>
-      </c>
-      <c r="J26">
-        <v>12</v>
-      </c>
-      <c r="K26">
-        <v>72</v>
-      </c>
-      <c r="M26" t="s">
-        <v>21</v>
-      </c>
-      <c r="N26" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="O26" t="s">
-        <v>44</v>
-      </c>
-      <c r="P26">
-        <v>10</v>
-      </c>
-      <c r="Q26">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -2785,38 +2002,8 @@
       <c r="E27">
         <v>26</v>
       </c>
-      <c r="G27" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I27" t="s">
-        <v>25</v>
-      </c>
-      <c r="J27">
-        <v>12</v>
-      </c>
-      <c r="K27">
-        <v>73</v>
-      </c>
-      <c r="M27" t="s">
-        <v>21</v>
-      </c>
-      <c r="N27" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="O27" t="s">
-        <v>25</v>
-      </c>
-      <c r="P27">
-        <v>13</v>
-      </c>
-      <c r="Q27">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -2832,38 +2019,8 @@
       <c r="E28">
         <v>25</v>
       </c>
-      <c r="G28" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I28" t="s">
-        <v>23</v>
-      </c>
-      <c r="J28">
-        <v>12</v>
-      </c>
-      <c r="K28">
-        <v>74</v>
-      </c>
-      <c r="M28" t="s">
-        <v>21</v>
-      </c>
-      <c r="N28" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="O28" t="s">
-        <v>23</v>
-      </c>
-      <c r="P28">
-        <v>17</v>
-      </c>
-      <c r="Q28">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -2879,38 +2036,8 @@
       <c r="E29">
         <v>27</v>
       </c>
-      <c r="G29" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I29" t="s">
-        <v>22</v>
-      </c>
-      <c r="J29">
-        <v>12</v>
-      </c>
-      <c r="K29">
-        <v>75</v>
-      </c>
-      <c r="M29" t="s">
-        <v>21</v>
-      </c>
-      <c r="N29" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="O29" t="s">
-        <v>22</v>
-      </c>
-      <c r="P29">
-        <v>14</v>
-      </c>
-      <c r="Q29">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -2926,38 +2053,8 @@
       <c r="E30">
         <v>28</v>
       </c>
-      <c r="G30" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I30" t="s">
-        <v>24</v>
-      </c>
-      <c r="J30">
-        <v>12</v>
-      </c>
-      <c r="K30">
-        <v>76</v>
-      </c>
-      <c r="M30" t="s">
-        <v>21</v>
-      </c>
-      <c r="N30" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="O30" t="s">
-        <v>24</v>
-      </c>
-      <c r="P30">
-        <v>1</v>
-      </c>
-      <c r="Q30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>1</v>
       </c>
@@ -2973,38 +2070,8 @@
       <c r="E31">
         <v>30</v>
       </c>
-      <c r="G31" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I31" t="s">
-        <v>45</v>
-      </c>
-      <c r="J31">
-        <v>12</v>
-      </c>
-      <c r="K31">
-        <v>77</v>
-      </c>
-      <c r="M31" t="s">
-        <v>21</v>
-      </c>
-      <c r="N31" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="O31" t="s">
-        <v>45</v>
-      </c>
-      <c r="P31">
-        <v>1</v>
-      </c>
-      <c r="Q31">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>1</v>
       </c>
@@ -3020,38 +2087,8 @@
       <c r="E32">
         <v>17</v>
       </c>
-      <c r="G32" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I32" t="s">
-        <v>44</v>
-      </c>
-      <c r="J32">
-        <v>15</v>
-      </c>
-      <c r="K32">
-        <v>90</v>
-      </c>
-      <c r="M32" t="s">
-        <v>21</v>
-      </c>
-      <c r="N32" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="O32" t="s">
-        <v>44</v>
-      </c>
-      <c r="P32">
-        <v>10</v>
-      </c>
-      <c r="Q32">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>1</v>
       </c>
@@ -3067,38 +2104,8 @@
       <c r="E33">
         <v>14</v>
       </c>
-      <c r="G33" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I33" t="s">
-        <v>25</v>
-      </c>
-      <c r="J33">
-        <v>15</v>
-      </c>
-      <c r="K33">
-        <v>91</v>
-      </c>
-      <c r="M33" t="s">
-        <v>21</v>
-      </c>
-      <c r="N33" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="O33" t="s">
-        <v>25</v>
-      </c>
-      <c r="P33">
-        <v>13</v>
-      </c>
-      <c r="Q33">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -3114,38 +2121,8 @@
       <c r="E34">
         <v>13</v>
       </c>
-      <c r="G34" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I34" t="s">
-        <v>23</v>
-      </c>
-      <c r="J34">
-        <v>15</v>
-      </c>
-      <c r="K34">
-        <v>92</v>
-      </c>
-      <c r="M34" t="s">
-        <v>21</v>
-      </c>
-      <c r="N34" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="O34" t="s">
-        <v>23</v>
-      </c>
-      <c r="P34">
-        <v>17</v>
-      </c>
-      <c r="Q34">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>1</v>
       </c>
@@ -3161,38 +2138,8 @@
       <c r="E35">
         <v>15</v>
       </c>
-      <c r="G35" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I35" t="s">
-        <v>22</v>
-      </c>
-      <c r="J35">
-        <v>15</v>
-      </c>
-      <c r="K35">
-        <v>93</v>
-      </c>
-      <c r="M35" t="s">
-        <v>21</v>
-      </c>
-      <c r="N35" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="O35" t="s">
-        <v>22</v>
-      </c>
-      <c r="P35">
-        <v>14</v>
-      </c>
-      <c r="Q35">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>1</v>
       </c>
@@ -3208,38 +2155,8 @@
       <c r="E36">
         <v>16</v>
       </c>
-      <c r="G36" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I36" t="s">
-        <v>24</v>
-      </c>
-      <c r="J36">
-        <v>15</v>
-      </c>
-      <c r="K36">
-        <v>94</v>
-      </c>
-      <c r="M36" t="s">
-        <v>21</v>
-      </c>
-      <c r="N36" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="O36" t="s">
-        <v>24</v>
-      </c>
-      <c r="P36">
-        <v>1</v>
-      </c>
-      <c r="Q36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>1</v>
       </c>
@@ -3255,34 +2172,1228 @@
       <c r="E37">
         <v>18</v>
       </c>
-      <c r="G37" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H37" s="4" t="s">
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" t="s">
+        <v>44</v>
+      </c>
+      <c r="D38">
+        <v>7</v>
+      </c>
+      <c r="E38">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39">
+        <v>7</v>
+      </c>
+      <c r="E39">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40">
+        <v>7</v>
+      </c>
+      <c r="E40">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41">
+        <v>7</v>
+      </c>
+      <c r="E41">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" t="s">
+        <v>24</v>
+      </c>
+      <c r="D42">
+        <v>7</v>
+      </c>
+      <c r="E42">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43" t="s">
+        <v>45</v>
+      </c>
+      <c r="D43">
+        <v>7</v>
+      </c>
+      <c r="E43">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" t="s">
+        <v>44</v>
+      </c>
+      <c r="D44">
+        <v>5</v>
+      </c>
+      <c r="E44">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" t="s">
+        <v>25</v>
+      </c>
+      <c r="D45">
+        <v>5</v>
+      </c>
+      <c r="E45">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46" t="s">
+        <v>23</v>
+      </c>
+      <c r="D46">
+        <v>5</v>
+      </c>
+      <c r="E46">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47" t="s">
+        <v>22</v>
+      </c>
+      <c r="D47">
+        <v>5</v>
+      </c>
+      <c r="E47">
         <v>34</v>
       </c>
-      <c r="I37" t="s">
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48" t="s">
+        <v>24</v>
+      </c>
+      <c r="D48">
+        <v>5</v>
+      </c>
+      <c r="E48">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C49" t="s">
         <v>45</v>
       </c>
-      <c r="J37">
+      <c r="D49">
+        <v>5</v>
+      </c>
+      <c r="E49">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C50" t="s">
+        <v>44</v>
+      </c>
+      <c r="D50">
+        <v>3</v>
+      </c>
+      <c r="E50">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C51" t="s">
+        <v>25</v>
+      </c>
+      <c r="D51">
+        <v>3</v>
+      </c>
+      <c r="E51">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C52" t="s">
+        <v>23</v>
+      </c>
+      <c r="D52">
+        <v>3</v>
+      </c>
+      <c r="E52">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C53" t="s">
+        <v>22</v>
+      </c>
+      <c r="D53">
+        <v>3</v>
+      </c>
+      <c r="E53">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C54" t="s">
+        <v>24</v>
+      </c>
+      <c r="D54">
+        <v>3</v>
+      </c>
+      <c r="E54">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C55" t="s">
+        <v>45</v>
+      </c>
+      <c r="D55">
+        <v>3</v>
+      </c>
+      <c r="E55">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C56" t="s">
+        <v>44</v>
+      </c>
+      <c r="D56">
+        <v>9</v>
+      </c>
+      <c r="E56">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C57" t="s">
+        <v>25</v>
+      </c>
+      <c r="D57">
+        <v>9</v>
+      </c>
+      <c r="E57">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C58" t="s">
+        <v>23</v>
+      </c>
+      <c r="D58">
+        <v>9</v>
+      </c>
+      <c r="E58">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C59" t="s">
+        <v>22</v>
+      </c>
+      <c r="D59">
+        <v>9</v>
+      </c>
+      <c r="E59">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C60" t="s">
+        <v>24</v>
+      </c>
+      <c r="D60">
+        <v>9</v>
+      </c>
+      <c r="E60">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C61" t="s">
+        <v>45</v>
+      </c>
+      <c r="D61">
+        <v>9</v>
+      </c>
+      <c r="E61">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C62" t="s">
+        <v>44</v>
+      </c>
+      <c r="D62">
+        <v>12</v>
+      </c>
+      <c r="E62">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C63" t="s">
+        <v>25</v>
+      </c>
+      <c r="D63">
+        <v>12</v>
+      </c>
+      <c r="E63">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C64" t="s">
+        <v>23</v>
+      </c>
+      <c r="D64">
+        <v>12</v>
+      </c>
+      <c r="E64">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C65" t="s">
+        <v>22</v>
+      </c>
+      <c r="D65">
+        <v>12</v>
+      </c>
+      <c r="E65">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C66" t="s">
+        <v>24</v>
+      </c>
+      <c r="D66">
+        <v>12</v>
+      </c>
+      <c r="E66">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C67" t="s">
+        <v>45</v>
+      </c>
+      <c r="D67">
+        <v>12</v>
+      </c>
+      <c r="E67">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C68" t="s">
+        <v>44</v>
+      </c>
+      <c r="D68">
         <v>15</v>
       </c>
-      <c r="K37">
+      <c r="E68">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C69" t="s">
+        <v>25</v>
+      </c>
+      <c r="D69">
+        <v>15</v>
+      </c>
+      <c r="E69">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C70" t="s">
+        <v>23</v>
+      </c>
+      <c r="D70">
+        <v>15</v>
+      </c>
+      <c r="E70">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C71" t="s">
+        <v>22</v>
+      </c>
+      <c r="D71">
+        <v>15</v>
+      </c>
+      <c r="E71">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C72" t="s">
+        <v>24</v>
+      </c>
+      <c r="D72">
+        <v>15</v>
+      </c>
+      <c r="E72">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C73" t="s">
+        <v>45</v>
+      </c>
+      <c r="D73">
+        <v>15</v>
+      </c>
+      <c r="E73">
         <v>95</v>
       </c>
-      <c r="M37" t="s">
-        <v>21</v>
-      </c>
-      <c r="N37" s="4" t="s">
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>21</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C74" t="s">
+        <v>44</v>
+      </c>
+      <c r="D74">
+        <v>10</v>
+      </c>
+      <c r="E74">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>21</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C75" t="s">
+        <v>25</v>
+      </c>
+      <c r="D75">
+        <v>13</v>
+      </c>
+      <c r="E75">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>21</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C76" t="s">
+        <v>23</v>
+      </c>
+      <c r="D76">
+        <v>17</v>
+      </c>
+      <c r="E76">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>21</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C77" t="s">
+        <v>22</v>
+      </c>
+      <c r="D77">
+        <v>14</v>
+      </c>
+      <c r="E77">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>21</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C78" t="s">
+        <v>24</v>
+      </c>
+      <c r="D78">
+        <v>1</v>
+      </c>
+      <c r="E78">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>21</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C79" t="s">
+        <v>45</v>
+      </c>
+      <c r="D79">
+        <v>1</v>
+      </c>
+      <c r="E79">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>21</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C80" t="s">
+        <v>44</v>
+      </c>
+      <c r="D80">
+        <v>10</v>
+      </c>
+      <c r="E80">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>21</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C81" t="s">
+        <v>25</v>
+      </c>
+      <c r="D81">
+        <v>13</v>
+      </c>
+      <c r="E81">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>21</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C82" t="s">
+        <v>23</v>
+      </c>
+      <c r="D82">
+        <v>17</v>
+      </c>
+      <c r="E82">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>21</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C83" t="s">
+        <v>22</v>
+      </c>
+      <c r="D83">
+        <v>14</v>
+      </c>
+      <c r="E83">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>21</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C84" t="s">
+        <v>24</v>
+      </c>
+      <c r="D84">
+        <v>1</v>
+      </c>
+      <c r="E84">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>21</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C85" t="s">
+        <v>45</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
+      </c>
+      <c r="E85">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>21</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C86" t="s">
+        <v>44</v>
+      </c>
+      <c r="D86">
+        <v>10</v>
+      </c>
+      <c r="E86">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>21</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C87" t="s">
+        <v>25</v>
+      </c>
+      <c r="D87">
+        <v>13</v>
+      </c>
+      <c r="E87">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>21</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C88" t="s">
+        <v>23</v>
+      </c>
+      <c r="D88">
+        <v>17</v>
+      </c>
+      <c r="E88">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>21</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C89" t="s">
+        <v>22</v>
+      </c>
+      <c r="D89">
+        <v>14</v>
+      </c>
+      <c r="E89">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>21</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C90" t="s">
+        <v>24</v>
+      </c>
+      <c r="D90">
+        <v>1</v>
+      </c>
+      <c r="E90">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>21</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C91" t="s">
+        <v>45</v>
+      </c>
+      <c r="D91">
+        <v>1</v>
+      </c>
+      <c r="E91">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>21</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C92" t="s">
+        <v>44</v>
+      </c>
+      <c r="D92">
+        <v>10</v>
+      </c>
+      <c r="E92">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>21</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C93" t="s">
+        <v>25</v>
+      </c>
+      <c r="D93">
+        <v>13</v>
+      </c>
+      <c r="E93">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>21</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C94" t="s">
+        <v>23</v>
+      </c>
+      <c r="D94">
+        <v>17</v>
+      </c>
+      <c r="E94">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>21</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C95" t="s">
+        <v>22</v>
+      </c>
+      <c r="D95">
+        <v>14</v>
+      </c>
+      <c r="E95">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>21</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C96" t="s">
+        <v>24</v>
+      </c>
+      <c r="D96">
+        <v>1</v>
+      </c>
+      <c r="E96">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>21</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C97" t="s">
+        <v>45</v>
+      </c>
+      <c r="D97">
+        <v>1</v>
+      </c>
+      <c r="E97">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>21</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C98" t="s">
+        <v>44</v>
+      </c>
+      <c r="D98">
+        <v>10</v>
+      </c>
+      <c r="E98">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>21</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C99" t="s">
+        <v>25</v>
+      </c>
+      <c r="D99">
+        <v>13</v>
+      </c>
+      <c r="E99">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>21</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C100" t="s">
+        <v>23</v>
+      </c>
+      <c r="D100">
+        <v>17</v>
+      </c>
+      <c r="E100">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>21</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C101" t="s">
+        <v>22</v>
+      </c>
+      <c r="D101">
+        <v>14</v>
+      </c>
+      <c r="E101">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>21</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C102" t="s">
+        <v>24</v>
+      </c>
+      <c r="D102">
+        <v>1</v>
+      </c>
+      <c r="E102">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>21</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C103" t="s">
+        <v>45</v>
+      </c>
+      <c r="D103">
+        <v>1</v>
+      </c>
+      <c r="E103">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>21</v>
+      </c>
+      <c r="B104" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="O37" t="s">
+      <c r="C104" t="s">
+        <v>44</v>
+      </c>
+      <c r="D104">
+        <v>10</v>
+      </c>
+      <c r="E104">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>21</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C105" t="s">
+        <v>25</v>
+      </c>
+      <c r="D105">
+        <v>13</v>
+      </c>
+      <c r="E105">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>21</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C106" t="s">
+        <v>23</v>
+      </c>
+      <c r="D106">
+        <v>17</v>
+      </c>
+      <c r="E106">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>21</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C107" t="s">
+        <v>22</v>
+      </c>
+      <c r="D107">
+        <v>14</v>
+      </c>
+      <c r="E107">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>21</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C108" t="s">
+        <v>24</v>
+      </c>
+      <c r="D108">
+        <v>1</v>
+      </c>
+      <c r="E108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>21</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C109" t="s">
         <v>45</v>
       </c>
-      <c r="P37">
-        <v>1</v>
-      </c>
-      <c r="Q37">
+      <c r="D109">
+        <v>1</v>
+      </c>
+      <c r="E109">
         <v>2</v>
       </c>
     </row>

</xml_diff>